<commit_message>
Added JPM positive mentions
</commit_message>
<xml_diff>
--- a/BIRT Project/Recommendation Finance/Data Objects/Innovate.xlsx
+++ b/BIRT Project/Recommendation Finance/Data Objects/Innovate.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{96DA263D-5C13-45B8-BDC7-6EB920E142DB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
   <si>
     <t>company</t>
   </si>
@@ -123,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,11 +435,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,10 +1019,10 @@
         <v>5</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1038,10 +1039,10 @@
         <v>3</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1165,6 +1166,86 @@
       </c>
       <c r="F36">
         <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>4</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>